<commit_message>
added geoloc to xlsx and csv
</commit_message>
<xml_diff>
--- a/data/RestoAndMenu.xlsx
+++ b/data/RestoAndMenu.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\Hackathon\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="26835" windowHeight="13350" activeTab="1"/>
+    <workbookView xWindow="1620" yWindow="30" windowWidth="26840" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="Canteen" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="200">
   <si>
     <t>Adress</t>
   </si>
@@ -609,12 +614,22 @@
   </si>
   <si>
     <t>Reminder to self: Errors from here down :(</t>
+  </si>
+  <si>
+    <t>lattitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -644,8 +659,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,6 +672,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -703,7 +723,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,7 +758,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -950,18 +970,20 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -971,8 +993,14 @@
       <c r="C1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -982,8 +1010,14 @@
       <c r="C2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>50.843482999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.3825599999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -993,8 +1027,14 @@
       <c r="C3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>50.839899000000003</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4.3836139999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1004,8 +1044,14 @@
       <c r="C4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>50.814210000000003</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.4147379999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -1015,104 +1061,138 @@
       <c r="C5" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>50.841160000000002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4.370933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>50.84064</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.372045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>149</v>
       </c>
       <c r="B7" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>152</v>
       </c>
       <c r="B8" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>80</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>108</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1122,772 +1202,1082 @@
       <c r="C18" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>80</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>82</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>83</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>84</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>85</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>86</v>
       </c>
       <c r="B28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>87</v>
       </c>
       <c r="B29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>88</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>89</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>90</v>
       </c>
       <c r="B32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>91</v>
       </c>
       <c r="B33" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>92</v>
       </c>
       <c r="B34" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>93</v>
       </c>
       <c r="B35" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>94</v>
       </c>
       <c r="B36" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>95</v>
       </c>
       <c r="B37" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>96</v>
       </c>
       <c r="B38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>97</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>98</v>
       </c>
       <c r="B40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>99</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>100</v>
       </c>
       <c r="B42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>101</v>
       </c>
       <c r="B43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>102</v>
       </c>
       <c r="B44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>103</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>104</v>
       </c>
       <c r="B46" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>105</v>
       </c>
       <c r="B47" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>106</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>107</v>
       </c>
       <c r="B49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>108</v>
       </c>
       <c r="B50" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>109</v>
       </c>
       <c r="B51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>110</v>
       </c>
       <c r="B52" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>111</v>
       </c>
       <c r="B53" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>112</v>
       </c>
       <c r="B54" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>113</v>
       </c>
       <c r="B55" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>114</v>
       </c>
       <c r="B56" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>115</v>
       </c>
       <c r="B57" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>116</v>
       </c>
       <c r="B58" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>117</v>
       </c>
       <c r="B59" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>120</v>
       </c>
       <c r="B60" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>121</v>
       </c>
       <c r="B61" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>122</v>
       </c>
       <c r="B62" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>123</v>
       </c>
       <c r="B63" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>124</v>
       </c>
       <c r="B64" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>125</v>
       </c>
       <c r="B65" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>126</v>
       </c>
       <c r="B66" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>127</v>
       </c>
       <c r="B67" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>128</v>
       </c>
       <c r="B68" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+    </row>
+    <row r="109" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+    </row>
+    <row r="146" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G146" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G147" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G148" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G149" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G150" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G151" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G152" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G153" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G154" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G155" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G156" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G157" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G158" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G159" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G160" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G161" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G162" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G163" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G164" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G165" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G166" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G167" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G168" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G169" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G170" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G171" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G172" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G173" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G174" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G175" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G176" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G177" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G178" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G179" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G180" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G181" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G182" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G183" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G184" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G185" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G186" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G187" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G188" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G189" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G190" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G191" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G192" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G193" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G194" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G195" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G196" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G197" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G198" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G199" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G200" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G201" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G202" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G203" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G204" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G205" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G206" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G207" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G208" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G209" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G210" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G211" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G212" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G213" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G214" t="s">
         <v>148</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1896,20 +2286,20 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="42.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="30.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>167</v>
       </c>
@@ -1938,7 +2328,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -1967,7 +2357,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -1996,7 +2386,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -2025,7 +2415,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -2054,7 +2444,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -2068,7 +2458,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>168</v>
       </c>
@@ -2082,7 +2472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>168</v>
       </c>
@@ -2096,7 +2486,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>168</v>
       </c>
@@ -2110,7 +2500,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -2124,7 +2514,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>168</v>
       </c>
@@ -2138,7 +2528,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>168</v>
       </c>
@@ -2152,7 +2542,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>168</v>
       </c>
@@ -2166,7 +2556,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>168</v>
       </c>
@@ -2180,7 +2570,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>168</v>
       </c>
@@ -2194,7 +2584,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>168</v>
       </c>
@@ -2208,7 +2598,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>168</v>
       </c>
@@ -2222,7 +2612,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -2236,7 +2626,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>168</v>
       </c>
@@ -2250,7 +2640,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>169</v>
       </c>
@@ -2258,7 +2648,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>169</v>
       </c>
@@ -2266,7 +2656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>196</v>
       </c>
@@ -2274,7 +2664,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>196</v>
       </c>

</xml_diff>